<commit_message>
- OTree algorithm - small bug - results of experiments - experimenter.cpp with command arguments
</commit_message>
<xml_diff>
--- a/data/experiments/resultsDFA_R664_pots2.xlsx
+++ b/data/experiments/resultsDFA_R664_pots2.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="16035" windowHeight="7725"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="16035" windowHeight="7725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="resultsDFA_R664_pots2" sheetId="1" r:id="rId1"/>
     <sheet name="List1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">resultsDFA_R664_pots2!$A$1:$R$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">resultsDFA_R664_pots2!$A$1:$R$30</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="41">
   <si>
     <t>Correct</t>
   </si>
@@ -127,12 +126,30 @@
   </si>
   <si>
     <t>TeacherRL</t>
+  </si>
+  <si>
+    <t>ExtraStates:0+EQ</t>
+  </si>
+  <si>
+    <t>ExtraStates:0+EQ-tryExtend</t>
+  </si>
+  <si>
+    <t>ExtraStates:1+EQ-tryExtend</t>
+  </si>
+  <si>
+    <t>ExtraStates:0+EQ-tryExtend-sameInput</t>
+  </si>
+  <si>
+    <t>ExtraStates:1+EQ-tryExtend-sameInput</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -612,9 +629,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -958,11 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1079,7 +1096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1149,13 +1166,13 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>1551177</v>
+        <v>1551245</v>
       </c>
       <c r="G4">
-        <v>1551177</v>
+        <v>1551245</v>
       </c>
       <c r="H4">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I4">
         <v>18621477</v>
@@ -1185,7 +1202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1238,7 +1255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1291,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1344,7 +1361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1397,7 +1414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1450,7 +1467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1500,7 +1517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1600,7 +1617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1617,31 +1634,31 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>718433</v>
+        <v>71698</v>
       </c>
       <c r="G13">
-        <v>1455712</v>
+        <v>103079</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>463</v>
       </c>
       <c r="I13">
-        <v>8709253</v>
+        <v>788471</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>8709254</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>36359.835290000003</v>
+        <v>1457.9506389999999</v>
       </c>
       <c r="M13" t="s">
         <v>33</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O13">
         <v>11</v>
@@ -1670,37 +1687,37 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>2138390</v>
+        <v>718433</v>
       </c>
       <c r="G14">
-        <v>2138390</v>
+        <v>1455712</v>
       </c>
       <c r="H14">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="I14">
-        <v>26491470</v>
+        <v>8709253</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>28629860</v>
+        <v>8709254</v>
       </c>
       <c r="L14">
-        <v>83.243166000000002</v>
+        <v>36359.835290000003</v>
       </c>
       <c r="M14" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="N14" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P14" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R14" t="s">
         <v>21</v>
@@ -1723,37 +1740,37 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>3102418</v>
+        <v>69463</v>
       </c>
       <c r="G15">
-        <v>3102418</v>
+        <v>99702</v>
       </c>
       <c r="H15">
-        <v>65</v>
+        <v>469</v>
       </c>
       <c r="I15">
-        <v>44393330</v>
+        <v>760065</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>44414579</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>41.765298999999999</v>
+        <v>1359.3016439999999</v>
       </c>
       <c r="M15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="N15" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="P15" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R15" t="s">
         <v>21</v>
@@ -1776,37 +1793,37 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>1551177</v>
+        <v>727367</v>
       </c>
       <c r="G16">
-        <v>1551177</v>
+        <v>1424236</v>
       </c>
       <c r="H16">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>18621477</v>
+        <v>8744664</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>18642187</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>65.377505999999997</v>
+        <v>30311.110214</v>
       </c>
       <c r="M16" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="N16" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="O16">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="P16" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R16" t="s">
         <v>21</v>
@@ -1829,37 +1846,37 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>1508894</v>
+        <v>69081</v>
       </c>
       <c r="G17">
-        <v>1508894</v>
+        <v>88114</v>
       </c>
       <c r="H17">
-        <v>69</v>
+        <v>493</v>
       </c>
       <c r="I17">
-        <v>18065605</v>
+        <v>742776</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>18086854</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>43.482925000000002</v>
+        <v>871.65473699999995</v>
       </c>
       <c r="M17" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="O17">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R17" t="s">
         <v>21</v>
@@ -1882,37 +1899,37 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>1508956</v>
+        <v>741468</v>
       </c>
       <c r="G18">
-        <v>1508956</v>
+        <v>811487</v>
       </c>
       <c r="H18">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="I18">
-        <v>18065838</v>
+        <v>8192461</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>18087087</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>43.800854000000001</v>
+        <v>11996.342986</v>
       </c>
       <c r="M18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O18">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="P18" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R18" t="s">
         <v>21</v>
@@ -1935,34 +1952,34 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <v>7611924</v>
+        <v>2138390</v>
       </c>
       <c r="G19">
-        <v>7611924</v>
+        <v>2138390</v>
       </c>
       <c r="H19">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="I19">
-        <v>122546926</v>
+        <v>26491470</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>129437737</v>
+        <v>28629860</v>
       </c>
       <c r="L19">
-        <v>9.3621649999999992</v>
+        <v>83.243166000000002</v>
       </c>
       <c r="M19" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="O19">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P19" t="s">
         <v>35</v>
@@ -1988,34 +2005,34 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <v>1619814</v>
+        <v>3102418</v>
       </c>
       <c r="G20">
-        <v>1619814</v>
+        <v>3102418</v>
       </c>
       <c r="H20">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="I20">
-        <v>19997123</v>
+        <v>44393330</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>20895922</v>
+        <v>44414579</v>
       </c>
       <c r="L20">
-        <v>2.4256549999999999</v>
+        <v>41.765298999999999</v>
       </c>
       <c r="M20" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P20" t="s">
         <v>35</v>
@@ -2041,34 +2058,34 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>779505</v>
+        <v>1551177</v>
       </c>
       <c r="G21">
-        <v>779505</v>
+        <v>1551177</v>
       </c>
       <c r="H21">
-        <v>399</v>
+        <v>69</v>
       </c>
       <c r="I21">
-        <v>8998530</v>
+        <v>18621477</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>9057181</v>
+        <v>18642187</v>
       </c>
       <c r="L21">
-        <v>1.708234</v>
+        <v>65.377505999999997</v>
       </c>
       <c r="M21" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N21" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O21">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="P21" t="s">
         <v>35</v>
@@ -2094,31 +2111,34 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <v>152160</v>
+        <v>1508894</v>
       </c>
       <c r="G22">
-        <v>152160</v>
+        <v>1508894</v>
       </c>
       <c r="H22">
-        <v>663</v>
+        <v>69</v>
       </c>
       <c r="I22">
-        <v>1418922</v>
+        <v>18065605</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1571082</v>
+        <v>18086854</v>
       </c>
       <c r="L22">
-        <v>1.1029150000000001</v>
+        <v>43.482925000000002</v>
       </c>
       <c r="M22" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
       </c>
       <c r="O22">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P22" t="s">
         <v>35</v>
@@ -2144,31 +2164,34 @@
         <v>2</v>
       </c>
       <c r="F23">
-        <v>73537</v>
+        <v>1508956</v>
       </c>
       <c r="G23">
-        <v>73537</v>
+        <v>1508956</v>
       </c>
       <c r="H23">
-        <v>581</v>
+        <v>69</v>
       </c>
       <c r="I23">
-        <v>805264</v>
+        <v>18065838</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>827176</v>
+        <v>18087087</v>
       </c>
       <c r="L23">
-        <v>1.6042259999999999</v>
+        <v>43.800854000000001</v>
       </c>
       <c r="M23" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="N23" t="s">
+        <v>25</v>
       </c>
       <c r="O23">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="P23" t="s">
         <v>35</v>
@@ -2194,31 +2217,34 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <v>1385800</v>
+        <v>7611924</v>
       </c>
       <c r="G24">
-        <v>5184420</v>
+        <v>7611924</v>
       </c>
       <c r="H24">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I24">
-        <v>16278835</v>
+        <v>122546926</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>18178146</v>
+        <v>129437737</v>
       </c>
       <c r="L24">
-        <v>47.513852999999997</v>
+        <v>9.3621649999999992</v>
       </c>
       <c r="M24" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="N24" t="s">
+        <v>27</v>
       </c>
       <c r="O24">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P24" t="s">
         <v>35</v>
@@ -2244,34 +2270,34 @@
         <v>2</v>
       </c>
       <c r="F25">
-        <v>718433</v>
+        <v>1619814</v>
       </c>
       <c r="G25">
-        <v>1455712</v>
+        <v>1619814</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="I25">
-        <v>8709253</v>
+        <v>19997123</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>8709254</v>
+        <v>20895922</v>
       </c>
       <c r="L25">
-        <v>38639.075060000003</v>
+        <v>2.4256549999999999</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="N25" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="O25">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="P25" t="s">
         <v>35</v>
@@ -2280,32 +2306,286 @@
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>664</v>
+      </c>
+      <c r="D26">
+        <v>32</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>779505</v>
+      </c>
+      <c r="G26">
+        <v>779505</v>
+      </c>
+      <c r="H26">
+        <v>399</v>
+      </c>
+      <c r="I26">
+        <v>8998530</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>9057181</v>
+      </c>
+      <c r="L26">
+        <v>1.708234</v>
+      </c>
+      <c r="M26" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26">
+        <v>7</v>
+      </c>
+      <c r="P26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>664</v>
+      </c>
+      <c r="D27">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>152160</v>
+      </c>
+      <c r="G27">
+        <v>152160</v>
+      </c>
+      <c r="H27">
+        <v>663</v>
+      </c>
+      <c r="I27">
+        <v>1418922</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1571082</v>
+      </c>
+      <c r="L27">
+        <v>1.1029150000000001</v>
+      </c>
+      <c r="M27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27">
+        <v>8</v>
+      </c>
+      <c r="P27" t="s">
+        <v>35</v>
+      </c>
+      <c r="R27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>664</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>73537</v>
+      </c>
+      <c r="G28">
+        <v>73537</v>
+      </c>
+      <c r="H28">
+        <v>581</v>
+      </c>
+      <c r="I28">
+        <v>805264</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>827176</v>
+      </c>
+      <c r="L28">
+        <v>1.6042259999999999</v>
+      </c>
+      <c r="M28" t="s">
+        <v>31</v>
+      </c>
+      <c r="O28">
+        <v>9</v>
+      </c>
+      <c r="P28" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>664</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>1385800</v>
+      </c>
+      <c r="G29">
+        <v>5184420</v>
+      </c>
+      <c r="H29">
+        <v>41</v>
+      </c>
+      <c r="I29">
+        <v>16278835</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>18178146</v>
+      </c>
+      <c r="L29">
+        <v>47.513852999999997</v>
+      </c>
+      <c r="M29" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+      <c r="P29" t="s">
+        <v>35</v>
+      </c>
+      <c r="R29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>664</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>718433</v>
+      </c>
+      <c r="G30">
+        <v>1455712</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>8709253</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>8709254</v>
+      </c>
+      <c r="L30">
+        <v>38639.075060000003</v>
+      </c>
+      <c r="M30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" t="s">
+        <v>34</v>
+      </c>
+      <c r="O30">
+        <v>11</v>
+      </c>
+      <c r="P30" t="s">
+        <v>35</v>
+      </c>
+      <c r="R30" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R25">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="TeacherRL"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R30"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:D25"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2318,8 +2598,20 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>72</v>
       </c>
@@ -2332,8 +2624,45 @@
       <c r="D2">
         <v>2138390</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>68</v>
+      </c>
+      <c r="L2" s="2">
+        <f t="shared" ref="L2:L12" si="0">K2/K$14</f>
+        <v>8.5</v>
+      </c>
+      <c r="M2">
+        <v>25166790</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" ref="N2:N12" si="1">M2/M$14</f>
+        <v>2.8896611454507064</v>
+      </c>
+      <c r="O2">
+        <v>2031058</v>
+      </c>
+      <c r="P2" s="2">
+        <f t="shared" ref="P2:P12" si="2">O2/O$14</f>
+        <v>2.8270666854111659</v>
+      </c>
+      <c r="Q2">
+        <v>2031058</v>
+      </c>
+      <c r="R2" s="2">
+        <f t="shared" ref="R2:R12" si="3">Q2/Q$14</f>
+        <v>1.3952333978149525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>65</v>
       </c>
@@ -2346,8 +2675,45 @@
       <c r="D3">
         <v>3102418</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>64</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>44138601</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0680122623605035</v>
+      </c>
+      <c r="O3">
+        <v>3081168</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" si="2"/>
+        <v>4.2887339529225414</v>
+      </c>
+      <c r="Q3">
+        <v>3081168</v>
+      </c>
+      <c r="R3" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1166054824031129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>69</v>
       </c>
@@ -2360,8 +2726,45 @@
       <c r="D4">
         <v>1551177</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>68</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="M4">
+        <v>18621477</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1381256234030634</v>
+      </c>
+      <c r="O4">
+        <v>1551245</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1592062168636463</v>
+      </c>
+      <c r="Q4">
+        <v>1551245</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0656263052032271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>69</v>
       </c>
@@ -2374,8 +2777,45 @@
       <c r="D5">
         <v>1508894</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>69</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>8.625</v>
+      </c>
+      <c r="M5">
+        <v>18065605</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0743001724717378</v>
+      </c>
+      <c r="O5">
+        <v>1508894</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1002570872997204</v>
+      </c>
+      <c r="Q5">
+        <v>1508894</v>
+      </c>
+      <c r="R5" s="2">
+        <f t="shared" si="3"/>
+        <v>1.036533325273131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>69</v>
       </c>
@@ -2388,8 +2828,45 @@
       <c r="D6">
         <v>1508956</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>69</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>8.625</v>
+      </c>
+      <c r="M6">
+        <v>18065838</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0743269256272612</v>
+      </c>
+      <c r="O6">
+        <v>1508956</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1003433862308665</v>
+      </c>
+      <c r="Q6">
+        <v>1508956</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0365759161152754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>38</v>
       </c>
@@ -2402,8 +2879,45 @@
       <c r="D7">
         <v>7611924</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>36</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="M7">
+        <v>117889394</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="1"/>
+        <v>13.536108550297023</v>
+      </c>
+      <c r="O7">
+        <v>7335188</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="2"/>
+        <v>10.209982002497101</v>
+      </c>
+      <c r="Q7">
+        <v>7335188</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0389005517574903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>41</v>
       </c>
@@ -2416,8 +2930,45 @@
       <c r="D8">
         <v>1619814</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>41</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>5.125</v>
+      </c>
+      <c r="M8">
+        <v>19997123</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2960778610978463</v>
+      </c>
+      <c r="O8">
+        <v>1619814</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2546486589563677</v>
+      </c>
+      <c r="Q8">
+        <v>1619814</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1127297157679541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>399</v>
       </c>
@@ -2430,8 +2981,45 @@
       <c r="D9">
         <v>779505</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>399</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>49.875</v>
+      </c>
+      <c r="M9">
+        <v>8997911</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0331438299013704</v>
+      </c>
+      <c r="O9">
+        <v>779448</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0849278916753546</v>
+      </c>
+      <c r="Q9">
+        <v>779448</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.53544107625684201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>663</v>
       </c>
@@ -2444,8 +3032,42 @@
       <c r="D10">
         <v>152160</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>661</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>82.625</v>
+      </c>
+      <c r="M10">
+        <v>1416183</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1626067126537718</v>
+      </c>
+      <c r="O10">
+        <v>151821</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.2113224197663526</v>
+      </c>
+      <c r="Q10">
+        <v>151821</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10429329427798906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>581</v>
       </c>
@@ -2458,8 +3080,42 @@
       <c r="D11">
         <v>73537</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>580</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="M11">
+        <v>805147</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="1"/>
+        <v>9.2447308626813343E-2</v>
+      </c>
+      <c r="O11">
+        <v>73523</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10233800507493392</v>
+      </c>
+      <c r="Q11">
+        <v>73523</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0506556241893999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>41</v>
       </c>
@@ -2472,8 +3128,42 @@
       <c r="D12">
         <v>1385800</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>41</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>5.125</v>
+      </c>
+      <c r="M12">
+        <v>16278835</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8691425085480924</v>
+      </c>
+      <c r="O12">
+        <v>1385800</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9289203029370867</v>
+      </c>
+      <c r="Q12">
+        <v>1385800</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.95197401683849547</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2486,230 +3176,450 @@
       <c r="D13">
         <v>718433</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13">
+        <v>11</v>
+      </c>
+      <c r="K13">
+        <v>463</v>
+      </c>
+      <c r="L13" s="2">
+        <f>K13/K$14</f>
+        <v>57.875</v>
+      </c>
+      <c r="M13">
+        <v>788471</v>
+      </c>
+      <c r="N13" s="2">
+        <f>M13/M$14</f>
+        <v>9.0532563470139174E-2</v>
+      </c>
+      <c r="O13">
+        <v>71698</v>
+      </c>
+      <c r="P13" s="2">
+        <f>O13/O$14</f>
+        <v>9.9797754279104658E-2</v>
+      </c>
+      <c r="Q13">
+        <v>103079</v>
+      </c>
+      <c r="R13" s="2">
+        <f>Q13/Q$14</f>
+        <v>7.0810022861664948E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>8709253</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>718433</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1455712</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>A2/A$13</f>
         <v>9</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ref="B15:D15" si="0">B2/B$13</f>
+        <f t="shared" ref="B15:D15" si="4">B2/B$13</f>
         <v>1.4689650150579237</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.0417614461309137</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.9764640544073004</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15">
+        <v>469</v>
+      </c>
+      <c r="L15" s="2">
+        <f>K15/K$14</f>
+        <v>58.625</v>
+      </c>
+      <c r="M15">
+        <v>760065</v>
+      </c>
+      <c r="N15" s="2">
+        <f>M15/M$14</f>
+        <v>8.7270974904506735E-2</v>
+      </c>
+      <c r="O15">
+        <v>69463</v>
+      </c>
+      <c r="P15" s="2">
+        <f>O15/O$14</f>
+        <v>9.6686817003116501E-2</v>
+      </c>
+      <c r="Q15">
+        <v>99702</v>
+      </c>
+      <c r="R15" s="2">
+        <f>Q15/Q$14</f>
+        <v>6.8490195862917935E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" ref="A16:D16" si="1">A3/A$13</f>
+        <f t="shared" ref="A16:D16" si="5">A3/A$13</f>
         <v>8.125</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.1312031500736408</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5.0972603505719718</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4.3183122156137035</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" ref="L16:L18" si="6">K16/K$14</f>
+        <v>0.5</v>
+      </c>
+      <c r="M16">
+        <v>8744664</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" ref="N16:N18" si="7">M16/M$14</f>
+        <v>1.0040659055374783</v>
+      </c>
+      <c r="O16">
+        <v>727367</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" ref="P16:P18" si="8">O16/O$14</f>
+        <v>1.0124353975944869</v>
+      </c>
+      <c r="Q16">
+        <v>1424236</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16:R18" si="9">Q16/Q$14</f>
+        <v>0.97837759117188017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" ref="A17:D17" si="2">A4/A$13</f>
+        <f t="shared" ref="A17:D17" si="10">A4/A$13</f>
         <v>8.625</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.0655795926666813</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.1381256234030634</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.1591115664230345</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17">
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <v>493</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="6"/>
+        <v>61.625</v>
+      </c>
+      <c r="M17">
+        <v>742776</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="7"/>
+        <v>8.5285844836520422E-2</v>
+      </c>
+      <c r="O17">
+        <v>69081</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="8"/>
+        <v>9.6155104233797722E-2</v>
+      </c>
+      <c r="Q17">
+        <v>88114</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="9"/>
+        <v>6.0529830076278823E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" ref="A18:D18" si="3">A5/A$13</f>
+        <f t="shared" ref="A18:D18" si="11">A5/A$13</f>
         <v>8.625</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>1.036533325273131</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2.0743001724717378</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2.1002570872997204</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="6"/>
+        <v>1.125</v>
+      </c>
+      <c r="M18">
+        <v>8192461</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="7"/>
+        <v>0.94066173069033587</v>
+      </c>
+      <c r="O18">
+        <v>741468</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0320628367572202</v>
+      </c>
+      <c r="Q18">
+        <v>811487</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="9"/>
+        <v>0.55745023740959754</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" ref="A19:D19" si="4">A6/A$13</f>
+        <f t="shared" ref="A19:D19" si="12">A6/A$13</f>
         <v>8.625</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.0365759161152754</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.0743269256272612</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.1003433862308665</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" ref="A20:D20" si="5">A7/A$13</f>
+        <f t="shared" ref="A20:D20" si="13">A7/A$13</f>
         <v>4.75</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>5.2290040887208455</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>14.070888283989454</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>10.595175889748941</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" ref="A21:D21" si="6">A8/A$13</f>
+        <f t="shared" ref="A21:D21" si="14">A8/A$13</f>
         <v>5.125</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>1.1127297157679541</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>2.2960778610978463</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>2.2546486589563677</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" ref="A22:D22" si="7">A9/A$13</f>
+        <f t="shared" ref="A22:D22" si="15">A9/A$13</f>
         <v>49.875</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0.53548023235365239</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>1.0332149037351424</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>1.0850072310152792</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" ref="A23:D23" si="8">A10/A$13</f>
+        <f t="shared" ref="A23:D23" si="16">A10/A$13</f>
         <v>82.875</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.10452617001165065</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.16292120575668201</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.21179428005116691</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" ref="A24:D24" si="9">A11/A$13</f>
+        <f t="shared" ref="A24:D24" si="17">A11/A$13</f>
         <v>72.625</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>5.051617352882988E-2</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>9.2460742614779934E-2</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0.10235749193035398</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" ref="A25:D25" si="10">A12/A$13</f>
+        <f t="shared" ref="A25:D25" si="18">A12/A$13</f>
         <v>5.125</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.5614324811501175</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>1.8691425085480924</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>1.9289203029370867</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" ref="A26:D26" si="11">A13/A$13</f>
+        <f t="shared" ref="A26:D26" si="19">A13/A$13</f>
         <v>1</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>

</xml_diff>